<commit_message>
addeed lowe edd folfer
</commit_message>
<xml_diff>
--- a/lowe/edd/data/ALAMEHWS.xlsx
+++ b/lowe/edd/data/ALAMEHWS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13950" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1367,14 +1367,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:JH53"/>
+  <dimension ref="A1:JI53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -1384,12 +1384,12 @@
     <col min="9" max="114" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>44456.697581018518</v>
+        <v>44491.610081018516</v>
       </c>
     </row>
-    <row r="2" spans="1:268" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:269" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1399,14 +1399,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1414,12 +1414,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:269" x14ac:dyDescent="0.2">
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -2234,11 +2234,14 @@
       <c r="JG8" s="8">
         <v>44378</v>
       </c>
-      <c r="JH8" s="9">
+      <c r="JH8" s="8">
         <v>44409</v>
       </c>
+      <c r="JI8" s="9">
+        <v>44440</v>
+      </c>
     </row>
-    <row r="9" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -3039,10 +3042,13 @@
         <v>811500</v>
       </c>
       <c r="JH9" s="11">
-        <v>807100</v>
+        <v>806400</v>
+      </c>
+      <c r="JI9" s="11">
+        <v>805200</v>
       </c>
     </row>
-    <row r="10" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -3843,10 +3849,13 @@
         <v>759100</v>
       </c>
       <c r="JH10" s="11">
-        <v>757000</v>
+        <v>756200</v>
+      </c>
+      <c r="JI10" s="11">
+        <v>763000</v>
       </c>
     </row>
-    <row r="11" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -4647,10 +4656,13 @@
         <v>52400</v>
       </c>
       <c r="JH11" s="11">
-        <v>50000</v>
+        <v>50200</v>
+      </c>
+      <c r="JI11" s="11">
+        <v>42200</v>
       </c>
     </row>
-    <row r="12" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -5453,8 +5465,11 @@
       <c r="JH12" s="12">
         <v>6.2E-2</v>
       </c>
+      <c r="JI12" s="12">
+        <v>5.1999999999999998E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -6234,7 +6249,7 @@
         <v>750900</v>
       </c>
     </row>
-    <row r="14" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -7014,7 +7029,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>10</v>
       </c>
@@ -7794,7 +7809,7 @@
         <v>750300</v>
       </c>
     </row>
-    <row r="16" spans="1:268" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:269" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
add november data release
</commit_message>
<xml_diff>
--- a/lowe/edd/data/ALAMEHWS.xlsx
+++ b/lowe/edd/data/ALAMEHWS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\LMIDATA AUTOCES\Published Data NAICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\LMIDATA AUTOCES\Published Data NAICS\Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13950" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1367,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:JI53"/>
+  <dimension ref="A1:JJ53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1384,12 +1384,12 @@
     <col min="9" max="114" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>44491.610081018516</v>
+        <v>44519.49428240741</v>
       </c>
     </row>
-    <row r="2" spans="1:269" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:270" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1399,14 +1399,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1414,12 +1414,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:270" x14ac:dyDescent="0.2">
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -2237,11 +2237,14 @@
       <c r="JH8" s="8">
         <v>44409</v>
       </c>
-      <c r="JI8" s="9">
+      <c r="JI8" s="8">
         <v>44440</v>
       </c>
+      <c r="JJ8" s="9">
+        <v>44470</v>
+      </c>
     </row>
-    <row r="9" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -3045,10 +3048,13 @@
         <v>806400</v>
       </c>
       <c r="JI9" s="11">
-        <v>805200</v>
+        <v>807100</v>
+      </c>
+      <c r="JJ9" s="11">
+        <v>809500</v>
       </c>
     </row>
-    <row r="10" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -3852,10 +3858,13 @@
         <v>756200</v>
       </c>
       <c r="JI10" s="11">
-        <v>763000</v>
+        <v>764800</v>
+      </c>
+      <c r="JJ10" s="11">
+        <v>769400</v>
       </c>
     </row>
-    <row r="11" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -4659,10 +4668,13 @@
         <v>50200</v>
       </c>
       <c r="JI11" s="11">
-        <v>42200</v>
+        <v>42300</v>
+      </c>
+      <c r="JJ11" s="11">
+        <v>40100</v>
       </c>
     </row>
-    <row r="12" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -5468,8 +5480,11 @@
       <c r="JI12" s="12">
         <v>5.1999999999999998E-2</v>
       </c>
+      <c r="JJ12" s="12">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="13" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -6249,7 +6264,7 @@
         <v>750900</v>
       </c>
     </row>
-    <row r="14" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -7029,7 +7044,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>10</v>
       </c>
@@ -7809,7 +7824,7 @@
         <v>750300</v>
       </c>
     </row>
-    <row r="16" spans="1:269" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:270" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>11</v>
       </c>

</xml_diff>